<commit_message>
Fix data entry errors
</commit_message>
<xml_diff>
--- a/2025 Fall Post-Season Tournament (Nov 21).xlsx
+++ b/2025 Fall Post-Season Tournament (Nov 21).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sbclaude\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C36F61-A5D6-4134-BD9A-3142C112C2F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2525EC57-998E-4E2F-A3CF-D169CE21AA8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="84">
   <si>
     <t>Champions</t>
   </si>
@@ -131,22 +131,13 @@
 December 3</t>
   </si>
   <si>
-    <t>#8  Bad News Bears</t>
-  </si>
-  <si>
     <t>#12 Clippers</t>
   </si>
   <si>
     <t>#7 Norsemen</t>
   </si>
   <si>
-    <t>#10 Stars</t>
-  </si>
-  <si>
     <t>#6 Shorebirds</t>
-  </si>
-  <si>
-    <t>#11 The Sandlot</t>
   </si>
   <si>
     <t>Semi-Finals
@@ -316,14 +307,35 @@
     <t>#4 Rebels</t>
   </si>
   <si>
-    <t>#5 Warhawks</t>
-  </si>
-  <si>
-    <t>#9 Lightning Strikes</t>
-  </si>
-  <si>
     <t>First Round
 November 26</t>
+  </si>
+  <si>
+    <t>#8  Bad News Bears 16</t>
+  </si>
+  <si>
+    <t>#9 Lightning Strikes 9</t>
+  </si>
+  <si>
+    <t># 8 Bad News Bears</t>
+  </si>
+  <si>
+    <t>#5 Warhawks 10</t>
+  </si>
+  <si>
+    <t>#12 Clippers 20</t>
+  </si>
+  <si>
+    <t>#7 Norsemen 30</t>
+  </si>
+  <si>
+    <t>#10 Stars 25</t>
+  </si>
+  <si>
+    <t>#6 Shorebirds 9</t>
+  </si>
+  <si>
+    <t>#11 The Sandlot 7</t>
   </si>
 </sst>
 </file>
@@ -1266,31 +1278,31 @@
     </row>
     <row r="4" spans="2:18" ht="21" thickBot="1">
       <c r="B4" s="49" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C4" s="49" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D4" s="49" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E4" s="49" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F4" s="49" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G4" s="49" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H4" s="49" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I4" s="49" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J4" s="49" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K4" s="48"/>
       <c r="L4" s="48"/>
@@ -1303,7 +1315,7 @@
     </row>
     <row r="5" spans="2:18" ht="30" customHeight="1" thickBot="1">
       <c r="B5" s="45" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C5" s="44">
         <v>17</v>
@@ -1318,7 +1330,7 @@
         <v>0.76200000000000001</v>
       </c>
       <c r="G5" s="44" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H5" s="44">
         <v>346</v>
@@ -1342,7 +1354,7 @@
     </row>
     <row r="6" spans="2:18" ht="30" customHeight="1" thickBot="1">
       <c r="B6" s="47" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C6" s="46">
         <v>16</v>
@@ -1357,7 +1369,7 @@
         <v>0.76200000000000001</v>
       </c>
       <c r="G6" s="46" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H6" s="46">
         <v>352</v>
@@ -1381,7 +1393,7 @@
     </row>
     <row r="7" spans="2:18" ht="30" customHeight="1" thickBot="1">
       <c r="B7" s="45" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C7" s="44">
         <v>13</v>
@@ -1420,7 +1432,7 @@
     </row>
     <row r="8" spans="2:18" ht="30" customHeight="1" thickBot="1">
       <c r="B8" s="47" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C8" s="46">
         <v>12</v>
@@ -1450,7 +1462,7 @@
         <v>5</v>
       </c>
       <c r="L8" s="54" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="M8" s="55"/>
       <c r="N8" s="55"/>
@@ -1461,7 +1473,7 @@
     </row>
     <row r="9" spans="2:18" ht="30" customHeight="1" thickBot="1">
       <c r="B9" s="45" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C9" s="44">
         <v>12</v>
@@ -1500,7 +1512,7 @@
     </row>
     <row r="10" spans="2:18" ht="30" customHeight="1" thickBot="1">
       <c r="B10" s="47" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C10" s="46">
         <v>10</v>
@@ -1539,7 +1551,7 @@
     </row>
     <row r="11" spans="2:18" ht="30" customHeight="1" thickBot="1">
       <c r="B11" s="45" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C11" s="44">
         <v>9</v>
@@ -1569,7 +1581,7 @@
         <v>9</v>
       </c>
       <c r="L11" s="54" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="M11" s="55"/>
       <c r="N11" s="55"/>
@@ -1580,7 +1592,7 @@
     </row>
     <row r="12" spans="2:18" ht="30" customHeight="1" thickBot="1">
       <c r="B12" s="47" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C12" s="46">
         <v>9</v>
@@ -1619,7 +1631,7 @@
     </row>
     <row r="13" spans="2:18" ht="30" customHeight="1" thickBot="1">
       <c r="B13" s="45" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C13" s="44">
         <v>9</v>
@@ -1658,7 +1670,7 @@
     </row>
     <row r="14" spans="2:18" ht="30" customHeight="1" thickBot="1">
       <c r="B14" s="47" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C14" s="46">
         <v>9</v>
@@ -1697,7 +1709,7 @@
     </row>
     <row r="15" spans="2:18" ht="30" customHeight="1" thickBot="1">
       <c r="B15" s="45" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C15" s="44">
         <v>8</v>
@@ -1727,7 +1739,7 @@
         <v>11</v>
       </c>
       <c r="L15" s="54" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="M15" s="55"/>
       <c r="N15" s="55"/>
@@ -1738,7 +1750,7 @@
     </row>
     <row r="16" spans="2:18" ht="30" customHeight="1">
       <c r="B16" s="42" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C16" s="41">
         <v>8</v>
@@ -1840,37 +1852,37 @@
   <sheetData>
     <row r="5" spans="2:19">
       <c r="C5" s="50" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D5" s="50" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E5" s="50" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F5" s="50" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G5" s="50" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H5" s="50" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="2:19">
       <c r="B6" s="50" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C6" s="50"/>
       <c r="D6" s="51" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E6" s="52" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F6" s="52" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G6" s="50">
         <v>3</v>
@@ -1917,13 +1929,13 @@
       <c r="B7" s="50"/>
       <c r="C7" s="50"/>
       <c r="D7" s="51" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E7" s="52" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F7" s="52" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G7" s="50"/>
       <c r="H7" s="50"/>
@@ -2017,17 +2029,17 @@
     </row>
     <row r="11" spans="2:19">
       <c r="B11" s="50" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C11" s="52" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D11" s="50"/>
       <c r="E11" s="52" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F11" s="52" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G11" s="50">
         <v>3</v>
@@ -2071,14 +2083,14 @@
     <row r="12" spans="2:19">
       <c r="B12" s="50"/>
       <c r="C12" s="52" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D12" s="50"/>
       <c r="E12" s="52" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F12" s="52" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G12" s="50"/>
       <c r="H12" s="50"/>
@@ -2189,17 +2201,17 @@
     </row>
     <row r="17" spans="2:19">
       <c r="B17" s="50" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C17" s="52" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D17" s="52" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E17" s="50"/>
       <c r="F17" s="52" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G17" s="50">
         <v>4</v>
@@ -2243,14 +2255,14 @@
     <row r="18" spans="2:19">
       <c r="B18" s="50"/>
       <c r="C18" s="52" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D18" s="52" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E18" s="50"/>
       <c r="F18" s="52" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G18" s="50"/>
       <c r="H18" s="50"/>
@@ -2327,16 +2339,16 @@
     </row>
     <row r="21" spans="2:19">
       <c r="B21" s="50" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C21" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="52" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="52" t="s">
         <v>60</v>
-      </c>
-      <c r="D21" s="52" t="s">
-        <v>54</v>
-      </c>
-      <c r="E21" s="52" t="s">
-        <v>63</v>
       </c>
       <c r="F21" s="50"/>
       <c r="G21" s="50">
@@ -2380,13 +2392,13 @@
     </row>
     <row r="22" spans="2:19">
       <c r="C22" s="52" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D22" s="52" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E22" s="52" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G22" s="50"/>
       <c r="H22" s="50"/>
@@ -2493,8 +2505,8 @@
   </sheetPr>
   <dimension ref="B1:M47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75"/>
@@ -2531,7 +2543,7 @@
     <row r="2" spans="2:13" ht="33.75">
       <c r="B2" s="24"/>
       <c r="C2" s="63" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D2" s="64"/>
       <c r="E2" s="64"/>
@@ -2579,7 +2591,7 @@
       <c r="B6" s="24"/>
       <c r="C6" s="11"/>
       <c r="D6" s="15" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E6" s="11"/>
       <c r="F6" s="15" t="s">
@@ -2587,11 +2599,11 @@
       </c>
       <c r="G6" s="11"/>
       <c r="H6" s="15" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I6" s="11"/>
       <c r="J6" s="15" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K6" s="11"/>
       <c r="M6" s="25"/>
@@ -2613,7 +2625,7 @@
       <c r="B8" s="24"/>
       <c r="C8" s="13"/>
       <c r="D8" s="32" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F8" s="12"/>
       <c r="M8" s="25"/>
@@ -2622,7 +2634,7 @@
       <c r="B9" s="24"/>
       <c r="D9" s="29"/>
       <c r="F9" s="20" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="M9" s="25"/>
     </row>
@@ -2648,7 +2660,7 @@
       <c r="B12" s="24"/>
       <c r="C12" s="10"/>
       <c r="D12" s="32" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="F12" s="72"/>
       <c r="G12" s="5"/>
@@ -2661,7 +2673,9 @@
       <c r="D13" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="14"/>
+      <c r="F13" s="14" t="s">
+        <v>77</v>
+      </c>
       <c r="H13" s="4"/>
       <c r="M13" s="25"/>
     </row>
@@ -2669,7 +2683,7 @@
       <c r="B14" s="24"/>
       <c r="C14" s="13"/>
       <c r="D14" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="20"/>
@@ -2688,7 +2702,7 @@
       <c r="B16" s="24"/>
       <c r="C16" s="13"/>
       <c r="D16" s="32" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F16" s="20"/>
       <c r="G16" s="6"/>
@@ -2702,7 +2716,7 @@
       <c r="C17" s="13"/>
       <c r="D17" s="37"/>
       <c r="F17" s="20" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="30"/>
@@ -2738,7 +2752,7 @@
       <c r="B20" s="24"/>
       <c r="C20" s="6"/>
       <c r="D20" s="32" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F20" s="72"/>
       <c r="J20" s="4"/>
@@ -2750,7 +2764,9 @@
       <c r="D21" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="F21" s="14"/>
+      <c r="F21" s="14" t="s">
+        <v>16</v>
+      </c>
       <c r="J21" s="4"/>
       <c r="M21" s="25"/>
     </row>
@@ -2758,7 +2774,7 @@
       <c r="B22" s="24"/>
       <c r="C22" s="13"/>
       <c r="D22" s="14" t="s">
-        <v>17</v>
+        <v>79</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="20"/>
@@ -2768,7 +2784,7 @@
     <row r="23" spans="2:13" ht="26.1" customHeight="1">
       <c r="B23" s="24"/>
       <c r="J23" s="72" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="K23" s="20" t="s">
         <v>0</v>
@@ -2779,7 +2795,7 @@
       <c r="B24" s="24"/>
       <c r="C24" s="13"/>
       <c r="D24" s="32" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F24" s="20"/>
       <c r="J24" s="72"/>
@@ -2790,7 +2806,7 @@
       <c r="B25" s="24"/>
       <c r="D25" s="29"/>
       <c r="F25" s="20" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J25" s="4"/>
       <c r="M25" s="25"/>
@@ -2819,7 +2835,7 @@
       <c r="B28" s="24"/>
       <c r="C28" s="6"/>
       <c r="D28" s="32" t="s">
-        <v>18</v>
+        <v>80</v>
       </c>
       <c r="F28" s="72"/>
       <c r="G28" s="5"/>
@@ -2834,7 +2850,9 @@
       <c r="D29" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="F29" s="14"/>
+      <c r="F29" s="32" t="s">
+        <v>17</v>
+      </c>
       <c r="H29" s="4"/>
       <c r="I29" s="8"/>
       <c r="J29" s="4"/>
@@ -2844,7 +2862,7 @@
       <c r="B30" s="24"/>
       <c r="C30" s="13"/>
       <c r="D30" s="14" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="E30" s="5"/>
       <c r="H30" s="4"/>
@@ -2865,7 +2883,7 @@
       <c r="B32" s="24"/>
       <c r="C32" s="13"/>
       <c r="D32" s="32" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F32" s="20"/>
       <c r="G32" s="10"/>
@@ -2878,7 +2896,7 @@
       <c r="C33" s="13"/>
       <c r="D33" s="29"/>
       <c r="F33" s="20" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G33" s="10"/>
       <c r="H33" s="33"/>
@@ -2909,7 +2927,7 @@
       <c r="B36" s="24"/>
       <c r="C36" s="10"/>
       <c r="D36" s="32" t="s">
-        <v>20</v>
+        <v>82</v>
       </c>
       <c r="F36" s="72"/>
       <c r="M36" s="25"/>
@@ -2920,14 +2938,16 @@
       <c r="D37" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="F37" s="14"/>
+      <c r="F37" s="32" t="s">
+        <v>18</v>
+      </c>
       <c r="M37" s="25"/>
     </row>
     <row r="38" spans="2:13" ht="26.1" customHeight="1">
       <c r="B38" s="24"/>
       <c r="C38" s="13"/>
       <c r="D38" s="14" t="s">
-        <v>21</v>
+        <v>83</v>
       </c>
       <c r="E38" s="5"/>
       <c r="F38" s="20"/>

</xml_diff>